<commit_message>
finish dev of production techs
</commit_message>
<xml_diff>
--- a/gameData/shared/MilitaryTechLevelUp.xlsx
+++ b/gameData/shared/MilitaryTechLevelUp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="1820" windowWidth="28720" windowHeight="14540" tabRatio="968" firstSheet="2" activeTab="15"/>
+    <workbookView xWindow="4820" yWindow="4020" windowWidth="28720" windowHeight="14540" tabRatio="968" firstSheet="2" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="infantry_infantry" sheetId="27" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="7">
   <si>
     <t>INT_level</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -128,6 +128,9 @@
   <si>
     <t>INT_coin</t>
     <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_buildTime</t>
   </si>
 </sst>
 </file>
@@ -271,7 +274,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="60">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -336,6 +339,42 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -349,7 +388,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="60">
+  <cellStyles count="96">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -382,6 +421,24 @@
     <cellStyle name="超链接" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -407,6 +464,24 @@
     <cellStyle name="访问过的超链接" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -856,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -867,7 +942,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -886,8 +961,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -906,8 +984,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -926,8 +1007,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -946,8 +1030,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -966,8 +1053,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -986,8 +1076,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1006,8 +1099,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1026,8 +1122,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1046,8 +1145,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1066,8 +1168,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1086,8 +1191,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1106,8 +1214,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1126,8 +1237,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1146,8 +1260,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1166,8 +1283,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1185,6 +1305,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -1201,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1212,7 +1335,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1231,8 +1354,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1251,8 +1377,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1271,8 +1400,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1291,8 +1423,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1311,8 +1446,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1331,8 +1469,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1351,8 +1492,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1371,8 +1515,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1391,8 +1538,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1411,8 +1561,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1431,8 +1584,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1451,8 +1607,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1471,8 +1630,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1491,8 +1653,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1511,8 +1676,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1530,6 +1698,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -1546,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1557,7 +1728,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1576,8 +1747,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1596,8 +1770,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1616,8 +1793,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1636,8 +1816,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1656,8 +1839,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1676,8 +1862,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1696,8 +1885,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1716,8 +1908,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1736,8 +1931,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1756,8 +1954,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1776,8 +1977,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1796,8 +2000,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1816,8 +2023,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1836,8 +2046,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1856,8 +2069,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1875,6 +2091,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -1891,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1902,7 +2121,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1921,8 +2140,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1941,8 +2163,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1961,8 +2186,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1981,8 +2209,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2001,8 +2232,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2021,8 +2255,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2041,8 +2278,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2061,8 +2301,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2081,8 +2324,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2101,8 +2347,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2121,8 +2370,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2141,8 +2393,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2161,8 +2416,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2181,8 +2439,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2201,8 +2462,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2220,6 +2484,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -2236,10 +2503,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2247,7 +2514,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2266,8 +2533,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2286,8 +2556,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2306,8 +2579,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2326,8 +2602,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2346,8 +2625,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2366,8 +2648,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2386,8 +2671,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2406,8 +2694,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2426,8 +2717,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2446,8 +2740,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2466,8 +2763,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2486,8 +2786,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2506,8 +2809,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2526,8 +2832,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2546,8 +2855,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2565,6 +2877,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -2581,10 +2896,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2592,7 +2907,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2611,8 +2926,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2631,8 +2949,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2651,8 +2972,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2671,8 +2995,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2691,8 +3018,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2711,8 +3041,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2731,8 +3064,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2751,8 +3087,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2771,8 +3110,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2791,8 +3133,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2811,8 +3156,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2831,8 +3179,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2851,8 +3202,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2871,8 +3225,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2891,8 +3248,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2910,6 +3270,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -2926,10 +3289,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2937,7 +3300,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2956,8 +3319,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2976,8 +3342,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2996,8 +3365,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3016,8 +3388,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3036,8 +3411,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3056,8 +3434,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3076,8 +3457,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3096,8 +3480,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3116,8 +3503,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3136,8 +3526,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3156,8 +3549,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3176,8 +3572,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3196,8 +3595,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3216,8 +3618,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3236,8 +3641,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3255,6 +3663,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -3271,10 +3682,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3282,7 +3693,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3301,8 +3712,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3321,8 +3735,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3341,8 +3758,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3361,8 +3781,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3381,8 +3804,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3401,8 +3827,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3421,8 +3850,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3441,8 +3873,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3461,8 +3896,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3481,8 +3919,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3501,8 +3942,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3521,8 +3965,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3541,8 +3988,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3561,8 +4011,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3581,8 +4034,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3600,6 +4056,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -3616,10 +4075,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3627,7 +4086,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3646,8 +4105,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3666,8 +4128,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3686,8 +4151,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3706,8 +4174,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3726,8 +4197,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3746,8 +4220,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3766,8 +4243,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3786,8 +4266,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3806,8 +4289,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3826,8 +4312,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3846,8 +4335,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3866,8 +4358,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3886,8 +4381,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3906,8 +4404,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3926,8 +4427,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3945,6 +4449,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -3961,10 +4468,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -3972,7 +4479,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3991,8 +4498,12 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4011,8 +4522,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4031,8 +4545,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4051,8 +4568,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4071,8 +4591,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4091,8 +4614,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4111,8 +4637,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4131,8 +4660,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4151,8 +4683,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4171,8 +4706,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4191,8 +4729,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4211,8 +4752,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4231,8 +4775,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4251,8 +4798,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4271,8 +4821,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4290,6 +4843,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -4306,10 +4862,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4317,7 +4873,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4336,8 +4892,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4356,8 +4915,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4376,8 +4938,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4396,8 +4961,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4416,8 +4984,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4436,8 +5007,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4456,8 +5030,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4476,8 +5053,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4496,8 +5076,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4516,8 +5099,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4536,8 +5122,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4556,8 +5145,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4576,8 +5168,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4596,8 +5191,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4616,8 +5214,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4635,6 +5236,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -4651,10 +5255,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4662,7 +5266,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4681,8 +5285,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4701,8 +5308,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4721,8 +5331,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4741,8 +5354,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4761,8 +5377,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4781,8 +5400,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4801,8 +5423,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4821,8 +5446,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4841,8 +5469,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4861,8 +5492,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4881,8 +5515,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4901,8 +5538,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4921,8 +5561,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4941,8 +5584,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4961,8 +5607,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4980,6 +5629,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -4996,10 +5648,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -5007,7 +5659,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5026,8 +5678,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5046,8 +5701,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5066,8 +5724,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5086,8 +5747,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5106,8 +5770,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -5126,8 +5793,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -5146,8 +5816,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -5166,8 +5839,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -5186,8 +5862,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -5206,8 +5885,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5226,8 +5908,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5246,8 +5931,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5266,8 +5954,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5286,8 +5977,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5306,8 +6000,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -5325,6 +6022,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -5341,10 +6041,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -5352,7 +6052,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5371,8 +6071,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5391,8 +6094,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5411,8 +6117,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5431,8 +6140,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5451,8 +6163,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -5471,8 +6186,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -5491,8 +6209,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -5511,8 +6232,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -5531,8 +6255,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -5551,8 +6278,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5571,8 +6301,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5591,8 +6324,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5611,8 +6347,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5631,8 +6370,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5651,8 +6393,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -5670,6 +6415,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -5686,10 +6434,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -5697,7 +6445,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5716,8 +6464,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5736,8 +6487,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5756,8 +6510,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5776,8 +6533,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5796,8 +6556,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -5816,8 +6579,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -5836,8 +6602,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -5856,8 +6625,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -5876,8 +6648,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -5896,8 +6671,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5916,8 +6694,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5936,8 +6717,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5956,8 +6740,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5976,8 +6763,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5996,8 +6786,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -6015,6 +6808,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>
@@ -6031,10 +6827,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -6042,7 +6838,7 @@
     <col min="1" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20" customHeight="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6061,8 +6857,11 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -6081,8 +6880,11 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1">
+      <c r="G2" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -6101,8 +6903,11 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
+      <c r="G3" s="1">
+        <v>34128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -6121,8 +6926,11 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="G4" s="1">
+        <v>45504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -6141,8 +6949,11 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1">
+      <c r="G5" s="1">
+        <v>56880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -6161,8 +6972,11 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1">
+      <c r="G6" s="1">
+        <v>68256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -6181,8 +6995,11 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1">
+      <c r="G7" s="1">
+        <v>91008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -6201,8 +7018,11 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1">
+      <c r="G8" s="1">
+        <v>113760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -6221,8 +7041,11 @@
       <c r="F9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1">
+      <c r="G9" s="1">
+        <v>136512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -6241,8 +7064,11 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
+      <c r="G10" s="1">
+        <v>159264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -6261,8 +7087,11 @@
       <c r="F11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
+      <c r="G11" s="1">
+        <v>182016</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -6281,8 +7110,11 @@
       <c r="F12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
+      <c r="G12" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -6301,8 +7133,11 @@
       <c r="F13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
+      <c r="G13" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -6321,8 +7156,11 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
+      <c r="G14" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -6341,8 +7179,11 @@
       <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
+      <c r="G15" s="1">
+        <v>204768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -6360,6 +7201,9 @@
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>204768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>